<commit_message>
first part of opportunity api implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/sheetfiles/SalesforceData.xlsx
+++ b/src/test/resources/sheetfiles/SalesforceData.xlsx
@@ -1,24 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13D89254-594F-428A-9736-720C49FEC2B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gui-automation\Salesforce-Wolfteam\src\test\resources\sheetfiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CCDEA9-AD27-4147-A214-1BA6E9ABA17E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Accounts" sheetId="1" r:id="rId1"/>
     <sheet name="Contacts" sheetId="2" r:id="rId2"/>
+    <sheet name="Opportunities" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Type</t>
   </si>
@@ -59,13 +63,55 @@
   </si>
   <si>
     <t>testing complete contact</t>
+  </si>
+  <si>
+    <t>TypeId</t>
+  </si>
+  <si>
+    <t>LeadSource</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>StageName</t>
+  </si>
+  <si>
+    <t>Probability</t>
+  </si>
+  <si>
+    <t>NextStep</t>
+  </si>
+  <si>
+    <t>Test Complete Opportunity</t>
+  </si>
+  <si>
+    <t>Test Basic Opportunity</t>
+  </si>
+  <si>
+    <t>New Customer</t>
+  </si>
+  <si>
+    <t>web</t>
+  </si>
+  <si>
+    <t>TODAY</t>
+  </si>
+  <si>
+    <t>Prospecting</t>
+  </si>
+  <si>
+    <t>This is a testing</t>
+  </si>
+  <si>
+    <t>CloseDate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -422,27 +468,27 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -450,7 +496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -463,6 +509,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -470,19 +517,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95426FC-9266-4CA3-AE73-9169E45E524F}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -491,7 +536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -499,7 +544,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -508,6 +553,109 @@
       </c>
       <c r="C3" t="s">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51929AAE-BF53-44F5-A8A3-D016B90BD2F9}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>